<commit_message>
Modified the test methods in send / request features
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\08-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933EF0FE-FB28-4F69-9169-C812BBE963DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FACAD9D-A7A1-4B31-B36D-F4CFD056C32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -97,9 +97,9 @@
 -pphoneNumDesc,
 -pcountry,
 -pphoneNumber,
--pphoneDescription,
+-pphoneVerificationDescription,
 -potp,
--pemailDesc,
+-pemailVerificationDescription,
 -pemail,
 -pemailDescription,
 -pnameDesc,
@@ -514,13 +514,14 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -561,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Prepared the test data and test scripts for Send/Request and Notifications feature
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\08-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FACAD9D-A7A1-4B31-B36D-F4CFD056C32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78E34F-8DA1-4D84-8B4A-6E56FBE65834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -110,6 +110,145 @@
 -plegalDesc,
 -pconfirmPinHeading,
 -ppin</t>
+  </si>
+  <si>
+    <t>Verify Notifications</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>testdata_3_0_customer.xls,notifications</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.LoginTest,
+testLogin,
+-pemail,
+-ppassword,
+-ppin</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testNotifications,
+-pnotificationsHeading,
+-ppassword,
+-ppin,
+-puserName</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testNotificationSend,
+-ppin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform Send transaction from Notifications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Deny in Notifications </t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testNotificationDeny,
+-pdenyMessage</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testRequestReminder,
+-preminderMessage</t>
+  </si>
+  <si>
+    <t>Verify Request Reminder</t>
+  </si>
+  <si>
+    <t>Verify Cancel in Requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform Send transaction from Requests </t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testRequestCancel,
+-pcancelMessage</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testRequestSend,
+-ppin</t>
+  </si>
+  <si>
+    <t>Verify Send Transaction</t>
+  </si>
+  <si>
+    <t>Verify Request Transaction</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testSend,
+-pname,
+-pchooseSendMethod,
+-paccountAddress,
+-pamount,
+-pmessage,
+-ppinHeading,
+-ppin</t>
+  </si>
+  <si>
+    <t>Verify Send With Invalid Data</t>
+  </si>
+  <si>
+    <t>Verify Send/Request  Navigations</t>
+  </si>
+  <si>
+    <t>Verify Send/Request with Insufficient funds</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testRequest,
+-pname,
+-pchooseRequestMethod,
+-paccountAddress,
+-pamount,
+-pmessage,
+-ppinHeading,
+-ppin,
+-prequestSuccHeading</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testSendWithInvalidData,
+-pname,
+-pamount,
+-perrMsg,
+-pelementName,
+-perrPopupHeading,
+-perrPopupDes</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testSendRequestNavigations,
+-pamount,
+-perrPopupHeading,
+-preloadAmtHeading,
+-paddPaymentHeading,
+-ppinHeading</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testSendWithInsufficientFunds,
+-pamount,
+-perrPopupHeading,
+-pwithoutPaymentMethod,
+-paddCardReloadHead,
+-preloadAmtHeading,
+-ppinHeading,
+-pcvv,
+-ppin</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -511,17 +650,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="8" max="8" width="35.85546875" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -590,6 +730,383 @@
       <c r="I2" s="9"/>
       <c r="J2" s="10"/>
     </row>
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified the test methods Of Customer portal v3.0
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\15-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74469FB9-6859-4B7D-A5E3-0F582DB6DA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7628B42E-FDC1-436F-98C5-CFCE9E2ED86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="147">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1292,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,65 +1344,63 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="229.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>46</v>
@@ -1425,14 +1423,12 @@
       <c r="H4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="I4" s="16"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>46</v>
@@ -1455,12 +1451,14 @@
       <c r="H5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>46</v>
@@ -1483,14 +1481,12 @@
       <c r="H6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="I6" s="16"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>46</v>
@@ -1513,12 +1509,14 @@
       <c r="H7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>46</v>
@@ -1533,18 +1531,20 @@
         <v>16</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>46</v>
@@ -1558,45 +1558,45 @@
       <c r="E9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>16</v>
+      <c r="F9" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>66</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>46</v>
@@ -1607,22 +1607,22 @@
       <c r="D11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="E11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>46</v>
@@ -1630,25 +1630,25 @@
       <c r="C12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="225" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>72</v>
+      <c r="H12" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>46</v>
@@ -1657,25 +1657,24 @@
         <v>49</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>46</v>
@@ -1683,26 +1682,26 @@
       <c r="C14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>15</v>
+      <c r="D14" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>74</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>79</v>
+    <row r="15" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>76</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>46</v>
@@ -1717,19 +1716,19 @@
         <v>16</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>46</v>
@@ -1744,47 +1743,45 @@
         <v>16</v>
       </c>
       <c r="F16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G17" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>88</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>46</v>
@@ -1793,7 +1790,7 @@
         <v>146</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>16</v>
@@ -1802,18 +1799,18 @@
         <v>16</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>46</v>
@@ -1822,27 +1819,27 @@
         <v>146</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="153" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>91</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>46</v>
@@ -1853,25 +1850,25 @@
       <c r="D20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="15">
-        <v>1</v>
+      <c r="E20" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="153" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>46</v>
@@ -1880,27 +1877,27 @@
         <v>146</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>46</v>
@@ -1909,27 +1906,27 @@
         <v>146</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="153" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="204" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>46</v>
@@ -1938,27 +1935,27 @@
         <v>146</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="153" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>46</v>
@@ -1967,27 +1964,27 @@
         <v>146</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="15">
-        <v>1</v>
-      </c>
-      <c r="F24" s="15">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>46</v>
@@ -1996,27 +1993,27 @@
         <v>146</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="15">
+        <v>2</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>46</v>
@@ -2027,25 +2024,25 @@
       <c r="D26" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="17" t="s">
+      <c r="E26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I26" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>46</v>
@@ -2063,18 +2060,18 @@
         <v>16</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>46</v>
@@ -2082,7 +2079,7 @@
       <c r="C28" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="14" t="s">
         <v>73</v>
       </c>
       <c r="E28" s="17" t="s">
@@ -2092,18 +2089,18 @@
         <v>16</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>46</v>
@@ -2121,18 +2118,18 @@
         <v>16</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>46</v>
@@ -2150,18 +2147,18 @@
         <v>16</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>46</v>
@@ -2179,7 +2176,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>86</v>
@@ -2188,9 +2185,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>46</v>
@@ -2207,19 +2204,19 @@
       <c r="F32" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="24" t="s">
-        <v>130</v>
+      <c r="G32" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>46</v>
@@ -2237,18 +2234,18 @@
         <v>16</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>46</v>
@@ -2266,18 +2263,18 @@
         <v>16</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>135</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>46</v>
@@ -2295,18 +2292,18 @@
         <v>16</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>86</v>
+        <v>136</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>46</v>
@@ -2324,70 +2321,73 @@
         <v>16</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I36" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+    <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="11" t="s">
+      <c r="D38" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H38" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>19</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>46</v>
@@ -2408,15 +2408,12 @@
         <v>20</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>46</v>
@@ -2440,12 +2437,12 @@
         <v>22</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>46</v>
@@ -2469,12 +2466,12 @@
         <v>22</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>46</v>
@@ -2498,12 +2495,12 @@
         <v>22</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>46</v>
@@ -2527,12 +2524,12 @@
         <v>22</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>46</v>
@@ -2547,7 +2544,7 @@
         <v>16</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G44" t="s">
         <v>20</v>
@@ -2556,12 +2553,12 @@
         <v>22</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>46</v>
@@ -2576,7 +2573,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G45" t="s">
         <v>20</v>
@@ -2585,12 +2582,12 @@
         <v>22</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>46</v>
@@ -2614,12 +2611,12 @@
         <v>22</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>46</v>
@@ -2643,12 +2640,12 @@
         <v>22</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>46</v>
@@ -2663,7 +2660,7 @@
         <v>16</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="G48" t="s">
         <v>20</v>
@@ -2672,7 +2669,7 @@
         <v>22</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -2733,403 +2730,32 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>49</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H74" s="8" t="s">
+    <row r="51" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" t="s">
-        <v>20</v>
-      </c>
-      <c r="H75" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>25</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" t="s">
-        <v>20</v>
-      </c>
-      <c r="H76" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I76" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" t="s">
-        <v>20</v>
-      </c>
-      <c r="H77" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I77" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>29</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" t="s">
-        <v>20</v>
-      </c>
-      <c r="H78" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I78" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>30</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" t="s">
-        <v>20</v>
-      </c>
-      <c r="H79" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>31</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" t="s">
-        <v>20</v>
-      </c>
-      <c r="H80" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I80" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G81" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I81" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>35</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" t="s">
-        <v>20</v>
-      </c>
-      <c r="H82" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I82" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>37</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G83" t="s">
-        <v>20</v>
-      </c>
-      <c r="H83" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I83" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>38</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G84" t="s">
-        <v>20</v>
-      </c>
-      <c r="H84" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>39</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G85" t="s">
-        <v>20</v>
-      </c>
-      <c r="H85" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I85" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>39</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G86" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I86" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>39</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G87" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I87" s="10" t="s">
+      <c r="I51" s="10" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Developed the test methods for Login Sessions feature in customer portal v3.0
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\15-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7628B42E-FDC1-436F-98C5-CFCE9E2ED86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08171918-34FD-463F-9FEC-2FC86FAF4D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="150">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -840,6 +840,28 @@
   </si>
   <si>
     <t>testdata_3_0_customer.xls,profile</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testLogInSessions,
+-ppinHeading,
+-ppin,
+-pexpHeading,
+-pdescription,
+-ppassword,
+-psubHeading,
+-pnewPassword,
+-pConfirmPassword,
+-psucessHeading,
+-psucessDesc,
+-pvalidateChangePassword,
+-pendSessnSucessHeading</t>
+  </si>
+  <si>
+    <t>Profile-Login Sessions</t>
+  </si>
+  <si>
+    <t>Verify Login Sessions in Profile</t>
   </si>
 </sst>
 </file>
@@ -914,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -977,6 +999,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,6 +2787,35 @@
         <v>44</v>
       </c>
     </row>
+    <row r="52" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified the test methods of customer portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\21-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953B577C-C439-44A1-BCB6-BBAF5D78DE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F461F7-6DED-41DF-BBE7-CBA929999F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="173">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1112,6 +1112,26 @@
 -pcardSucessDesc,
 -pbuyTokenHeading
 </t>
+  </si>
+  <si>
+    <t>Verify Edit Email with valid credentials</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditEmail,
+-ppinHeading,
+-pemail,
+-pnewEmail,
+-peditEmailHeading,
+-ppin,
+-pnewEmail,
+-pcurrentEmailVerification,
+-pcurrEmailVerifiDesc,
+-pnewEmailVerifiDesc,
+-pcode,
+-pnewEmailVerification,
+-psucessDesc,
+-psucessHeading</t>
   </si>
 </sst>
 </file>
@@ -1570,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,7 +2018,7 @@
         <v>169</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
@@ -2021,15 +2041,15 @@
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>49</v>
+    <row r="17" spans="1:10" ht="204" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>171</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>15</v>
@@ -2038,59 +2058,59 @@
         <v>16</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>51</v>
+        <v>84</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="153" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>16</v>
+      <c r="E18" s="15">
+        <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>87</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>16</v>
@@ -2099,17 +2119,18 @@
         <v>16</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>45</v>
@@ -2132,14 +2153,12 @@
       <c r="H20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="16" t="s">
-        <v>55</v>
-      </c>
+      <c r="I20" s="16"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>45</v>
@@ -2162,12 +2181,14 @@
       <c r="H21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>45</v>
@@ -2182,18 +2203,20 @@
         <v>16</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>45</v>
@@ -2207,98 +2230,103 @@
       <c r="E23" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="225" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>45</v>
@@ -2309,110 +2337,102 @@
       <c r="D27" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="E27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G30" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H30" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:10" ht="102" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I28" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="216.75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="153" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>86</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>45</v>
@@ -2423,25 +2443,25 @@
       <c r="D31" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="15">
-        <v>1</v>
+      <c r="E31" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>45</v>
@@ -2459,18 +2479,18 @@
         <v>16</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>45</v>
@@ -2488,18 +2508,18 @@
         <v>44</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="153" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>95</v>
+      <c r="A34" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>45</v>
@@ -2508,27 +2528,27 @@
         <v>138</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>89</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>45</v>
@@ -2537,27 +2557,27 @@
         <v>138</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="15">
-        <v>1</v>
-      </c>
-      <c r="F35" s="15">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>101</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>45</v>
@@ -2566,27 +2586,27 @@
         <v>138</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>104</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="153" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>95</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>45</v>
@@ -2597,25 +2617,25 @@
       <c r="D37" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="17" t="s">
+      <c r="E37" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I37" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I37" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>45</v>
@@ -2624,27 +2644,27 @@
         <v>138</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E38" s="15">
+        <v>1</v>
+      </c>
+      <c r="F38" s="15">
+        <v>2</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I38" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I38" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>45</v>
@@ -2652,28 +2672,28 @@
       <c r="C39" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="17" t="s">
+      <c r="E39" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="16" t="s">
-        <v>112</v>
+      <c r="I39" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>45</v>
@@ -2681,7 +2701,7 @@
       <c r="C40" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="14" t="s">
         <v>69</v>
       </c>
       <c r="E40" s="17" t="s">
@@ -2691,18 +2711,18 @@
         <v>16</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>45</v>
@@ -2710,7 +2730,7 @@
       <c r="C41" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="14" t="s">
         <v>69</v>
       </c>
       <c r="E41" s="17" t="s">
@@ -2720,18 +2740,18 @@
         <v>16</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>45</v>
@@ -2749,18 +2769,18 @@
         <v>16</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>45</v>
@@ -2777,19 +2797,19 @@
       <c r="F43" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="24" t="s">
-        <v>122</v>
+      <c r="G43" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>45</v>
@@ -2806,19 +2826,19 @@
       <c r="F44" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="24" t="s">
-        <v>125</v>
+      <c r="G44" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>127</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>45</v>
@@ -2835,19 +2855,19 @@
       <c r="F45" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>129</v>
+      <c r="G45" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>45</v>
@@ -2865,18 +2885,18 @@
         <v>16</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>45</v>
@@ -2894,128 +2914,131 @@
         <v>16</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>78</v>
       </c>
       <c r="I47" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="16" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+    <row r="51" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B51" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="11" t="s">
+      <c r="D51" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H51" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="52" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>18</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" t="s">
-        <v>19</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>28</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>45</v>
@@ -3036,15 +3059,12 @@
         <v>19</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>45</v>
@@ -3068,12 +3088,12 @@
         <v>21</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>45</v>
@@ -3097,12 +3117,12 @@
         <v>21</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>45</v>
@@ -3117,7 +3137,7 @@
         <v>16</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="G55" t="s">
         <v>19</v>
@@ -3126,12 +3146,12 @@
         <v>21</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>45</v>
@@ -3155,12 +3175,12 @@
         <v>21</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>45</v>
@@ -3184,12 +3204,12 @@
         <v>21</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>45</v>
@@ -3204,7 +3224,7 @@
         <v>16</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="G58" t="s">
         <v>19</v>
@@ -3213,12 +3233,12 @@
         <v>21</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>45</v>
@@ -3233,7 +3253,7 @@
         <v>16</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G59" t="s">
         <v>19</v>
@@ -3242,12 +3262,12 @@
         <v>21</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>45</v>
@@ -3262,7 +3282,7 @@
         <v>16</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G60" t="s">
         <v>19</v>
@@ -3271,12 +3291,12 @@
         <v>21</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>45</v>
@@ -3291,7 +3311,7 @@
         <v>16</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G61" t="s">
         <v>19</v>
@@ -3300,35 +3320,122 @@
         <v>21</v>
       </c>
       <c r="I61" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="63" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="14" t="s">
+      <c r="B65" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D65" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E62" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="26" t="s">
+      <c r="E65" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="G62" s="24" t="s">
+      <c r="G65" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="H62" s="19" t="s">
+      <c r="H65" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="I62" s="16" t="s">
+      <c r="I65" s="16" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Developed the Test Scripts for some features of customer portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\21-June-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\30-June-2023_v3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F461F7-6DED-41DF-BBE7-CBA929999F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F51CFE-7AE2-4A02-AFA7-A4C7C9729BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="218">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -471,124 +471,22 @@
 -pexpHeading</t>
   </si>
   <si>
-    <t>Verify Edit Email in Profile</t>
-  </si>
-  <si>
     <t>Profile-Edit Email</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testEditEmail,
--pexpHeading,
--pheading,
--pexpSubHeading,
--pexistingEmail,
--ppin,
--pEditEmail,
--pnewEmail,
--pemailVerificationHeading,
--pverificationText,
--pcode,
--pnewEmailVerificationHeading,
--pnewVerificationText,
--psucessDesc,
--psucessHeading</t>
-  </si>
-  <si>
-    <t>verify Edit Email with Invalid Data</t>
-  </si>
-  <si>
     <t>User Details</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testEditEmailWithInvalidData,
--puserDetailsHeading,
--ppinHeading,
--ppin,
--peditEmailHeading,
--pValidateEmailFields,
--pnewEmail,
--pvalidateErrorMessage,
--perrMsg,
--pelementName</t>
-  </si>
-  <si>
     <t>Verify Edit Email Field Validations and Navigation</t>
   </si>
   <si>
-    <t>Profile-Edit Email Field validations</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testEditEmailFieldValidations,
--expHeading,
--ppin,
--pemail,
--pcode,
--pnewEmailVerificationHeading</t>
-  </si>
-  <si>
-    <t>Verify Edit Phone Number in Profile</t>
-  </si>
-  <si>
     <t>Profile-Edit Phone Number</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testEditPhoneNumber,
--pexpHeading,
--pheading,
--psubHeading,
--pexistingPhoneNumber,
--ppin,
--peditPhoneHeading,
--pfillCountry,
--pphoneNumber,
--pphoneVerificationHeading,
--pverificationText,
--pcode,
--pnewPhoneVerificationHeading,
--pnewVerificationText</t>
-  </si>
-  <si>
-    <t>Verify Edit Phone Number Field Validations in Profile</t>
-  </si>
-  <si>
-    <t>Profile-Edit Phone Number Field Validations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coyni_mobile.tests.CustomerProfileTest,
-testEditPhoneNumberFieldValidations,
--pexpHeading,
--ppin,
--pfillCountry,
--pphoneNumber,
--pphoneNumbers,
--pcode,
--pnewPhoneVerificationHeading
-</t>
-  </si>
-  <si>
     <t>Verify Edit Address in Profile</t>
   </si>
   <si>
     <t>Profile-Edit Address</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testEditAddress,
--pexpHeading,
--pheading,
--psubHeading,
--pexistingAddress,
--peditAddressHeading,
--pfillCountry,
--paddline1,
--paddline2,
--pcity,
--pstate,
--pzipcode</t>
   </si>
   <si>
     <t>Verify Edit Address Field Validations and Navigation in Profile</t>
@@ -614,49 +512,16 @@
     <t>Profile-Preferences</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testPrefernces,
--expHeading,
--ptimeZones,
--ptoastMsg</t>
-  </si>
-  <si>
     <t>Verify Account Limits in Profile</t>
   </si>
   <si>
     <t>Profile-Account Limits</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testAccountLimits,
--pexpHeading,
--psendReqHeading,
--pbuyTokenHeading,
--pWithdrawTokenHeading</t>
-  </si>
-  <si>
-    <t>Verify Agreements in Profile</t>
-  </si>
-  <si>
-    <t>Profile-Agreements</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testAgreements,
--pheading</t>
-  </si>
-  <si>
     <t>Verify Wallet Fees in Profile</t>
   </si>
   <si>
     <t>Profile-Wallet Fees</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testWalletFees,
--pexpHeading,
--pbuyTokenHeading,
--pWithdrawTokenHeading</t>
   </si>
   <si>
     <t>Verify Reset Pincode in Profile</t>
@@ -684,12 +549,6 @@
     <t>Profile-Reset Pincode View</t>
   </si>
   <si>
-    <t>Verify FaceId in Profile</t>
-  </si>
-  <si>
-    <t>Profile-Face Id</t>
-  </si>
-  <si>
     <t>coyni_mobile.tests.CustomerProfileTest,
 testEnableTouchOrFaceID</t>
   </si>
@@ -698,20 +557,6 @@
   </si>
   <si>
     <t>Profile-Change Password</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testChangePassword,
--ppinHeading,
--ppin,
--pexpHeading,
--pdescription,
--ppassword,
--psubHeading,
--pnewPassword,
--pConfirmPassword,
--psucessHeading,
--psucessDesc</t>
   </si>
   <si>
     <t>Verify Change Password with Invalid Data</t>
@@ -758,38 +603,13 @@
 -pConfirmPassword</t>
   </si>
   <si>
-    <t>Verify GetHelp in Profile</t>
-  </si>
-  <si>
     <t>Profile-Get Help</t>
   </si>
   <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testGetHelp,
--pexpHeading,
--pdescription</t>
-  </si>
-  <si>
     <t>testdata_3_0_customer.xls,SignUp</t>
   </si>
   <si>
     <t>testdata_3_0_customer.xls,profile</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testLogInSessions,
--ppinHeading,
--ppin,
--pexpHeading,
--pdescription,
--ppassword,
--psubHeading,
--pnewPassword,
--pConfirmPassword,
--psucessHeading,
--psucessDesc,
--pvalidateChangePassword,
--pendSessnSucessHeading</t>
   </si>
   <si>
     <t>Profile-Login Sessions</t>
@@ -1064,6 +884,335 @@
     <t>Verify SignUp with Add Debit or Credit Card</t>
   </si>
   <si>
+    <t>Verify Edit Email with valid credentials</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditEmail,
+-ppinHeading,
+-pemail,
+-pnewEmail,
+-peditEmailHeading,
+-ppin,
+-pnewEmail,
+-pcurrentEmailVerification,
+-pcurrEmailVerifiDesc,
+-pnewEmailVerifiDesc,
+-pcode,
+-pnewEmailVerification,
+-psucessDesc,
+-psucessHeading</t>
+  </si>
+  <si>
+    <t>Verify Edit Phone Number with valid credentials</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditAddress,
+-pheading,
+-psubHeading,
+-peditAddressHeading,
+-pcountry,
+-paddLine1,
+-paddLine2,
+-pcity,
+-pstate,
+-pzipCode,
+-paddressDesc,
+-ptoastMsg</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditPhoneNumber,
+-ppinHeading,
+-pheading,
+-psubHeading,
+-pexistingPhoneNumber,
+-ppin,
+-peditPhoneHeading,
+-pcountry,
+-pphoneNumber,
+-pcurrPhVerifiHeading,
+-pverificationText,
+-pcode,
+-pnewPhoneVerificationHeading,
+-pnewVerificationText,
+-ptoastMsg</t>
+  </si>
+  <si>
+    <t>Verify Edit Phone Number Navigation view</t>
+  </si>
+  <si>
+    <t>Verify Edit Phone Number with invalid and field validations</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditPhoneNumberInvalidData,
+-ppinHeading,
+-pheading,
+-ppin,
+-pfogtPINHeadi,
+-peditPhoneHeading,
+-pcountry,
+-pphoneNumber,
+-pfieldEmail,
+-pemail,
+-pemailErrMsg,
+-pfieldPhoneNumber,
+-pphNumErrMsg,
+-pvalidateEmail</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditPhoneNumberNavigationView,
+-ppinHeading,
+-pheading,
+-ppin,
+-peditPhoneHeading,
+-pcountry,
+-pphoneNumber,
+-pcurrPhVerifiHeading,
+-pcode,
+-pnewPhoneVerificationHeading,
+-pinvalidCode,
+-pinvalidCodeMsg,
+-pfogtPINHeadi,
+-pfogtPINDesc,
+-pemail</t>
+  </si>
+  <si>
+    <t>Verify Edit Email with invalid and field validations</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditEmailNavigationView,
+-ppinHeading,
+-pheading,
+-ppin,
+-peditEmailHeading,
+-pcountry,
+-pnewEmail,
+-pcurrentEmailVerification,
+-pcode,
+-pnewEmailVerification,
+-pinvalidCode,
+-pinvalidCodeMsg,
+-pfogtPINHeadi,
+-pfogtPINDesc,
+-pemail</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditEmailInvalidData,
+-ppinHeading,
+-ppin,
+-pfogtPINHeadi,
+-peditEmailHeading,
+-pfieldEmail,
+-pemail,
+-pemailErrMsg,
+-pnewEmail</t>
+  </si>
+  <si>
+    <t>Verify Logout</t>
+  </si>
+  <si>
+    <t>Profile-Logout</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testLogout,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.CustomerProfileTest,
+testResetPincode,
+-ppinHeading,
+-ppin,
+-pchoosePinDesc,
+-pchoosePinHeading,
+-pconfirmPinHeading,
+-ptoastMsg,
+-pfogtPINHeadi,
+-pfogtPINDesc,
+-pemail
+</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testChangePassword,
+-ppinHeading,
+-ppin,
+-pcurrPwdHeading,
+-pcurrPwdDescription,
+-ppassword,
+-psubHeading,
+-pnewPassword,
+-pconfirmPassword,
+-psucessHeading,
+-psucessDesc,
+-pdescription</t>
+  </si>
+  <si>
+    <t>Verify Change Password Field validations and Navigation</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testChangePasswordNavigationView,
+-ppinHeading,
+-ppin,
+-pcurrPwdHeading,
+-ppassword,
+-psubHeading,
+-pfieldPassword,
+-pfogtPINHeadi,
+-pfogtPINDesc,
+-pemail</t>
+  </si>
+  <si>
+    <t>Verify Change Password with invalid data and validations</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testChangePasswordFieldValidations,
+-ppinHeading,
+-ppin,
+-pcurrPwdHeading,
+-pfieldCurrntPwd,
+-pcurrntPwdErrMsg,
+-ppassword,
+-pfieldPassword,
+-psubHeading,
+-ppwdErrorMsg,
+-pconfPwdErrMsg,
+-pfieldConfPwd</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testAccountLimits,
+-psubHeading,
+-psendReqHeading,
+-pbuyTokenHeading,
+-pwithdrawTokenHeading</t>
+  </si>
+  <si>
+    <t>Verify Get Help in Profile</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testGetHelp,
+-pgetHelpHeading,
+-pgetHelpDesc</t>
+  </si>
+  <si>
+    <t>Verify Touch ID in Profile</t>
+  </si>
+  <si>
+    <t>Profile-Touch ID</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testLogInSessions,
+-ppinHeading,
+-ppin,
+-pcurrPwdHeading,
+-pcurrPwdDescription,
+-ppassword,
+-psubHeading,
+-pnewPassword,
+-pconfirmPassword,
+-psucessHeading,
+-psucessDesc,
+-pdescription,
+-plogInSessionHeading,
+-pvalidateChangePassword,
+-pdeviceStatus,
+-pendSessnSucessHeading,
+-pendSessnHeading</t>
+  </si>
+  <si>
+    <t>Verify Agreements in Profile</t>
+  </si>
+  <si>
+    <t>Profile-Agreements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.CustomerProfileTest,
+testAgreements,
+-pagreementsHeading,
+-pprivacyHeading,
+-pagreeDocHeading,
+-ptermsHeading
+</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testPrefernces,
+-psubHeading,
+-ptimeZones,
+-ptoastMsg</t>
+  </si>
+  <si>
+    <t>Verify Edit Address with Invalid data and Navigation view</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditAddressFieldValidations,
+-pheading,
+-peditAddressHeading,
+-pcountry,
+-paddLine1,
+-paddLine2,
+-pcity,
+-pstate,
+-pzipCode,
+-paddLine1ErrMsg,
+-pcityErrMsg,
+-pzipCodeErrMsg</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testWalletFees,
+-psubHeading,
+-pbuyTokenHeading,
+-pwithdrawTokenHeading</t>
+  </si>
+  <si>
     <t xml:space="preserve">coyni_mobile.tests.SignUpTest,
 testSignUpWithAddDebitCreditCard,
 -pphoneNumDesc,
@@ -1109,36 +1258,234 @@
 -pcardSucessDescription,
 -paddPaymentHeading,
 -pbillingAddrHeading,
--pcardSucessDesc,
 -pbuyTokenHeading
 </t>
   </si>
   <si>
-    <t>Verify Edit Email with valid credentials</t>
+    <t>Verify Add Debit and Credit Card</t>
+  </si>
+  <si>
+    <t>Payment Methods</t>
+  </si>
+  <si>
+    <t>testdata_3_0_customer.xls,PaymentMethods</t>
+  </si>
+  <si>
+    <t>Buy Token - Debit Card</t>
+  </si>
+  <si>
+    <t>Verify Buy Token with New and Existing Debit and Credit Cards</t>
+  </si>
+  <si>
+    <t>testdata_3_0_customer.xls,buyTokens</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testDeleteCards,
+-ppaymentHeading,
+-pcardHeading,
+-premovePopUpHeading,
+-ptoastMsg</t>
+  </si>
+  <si>
+    <t>Verify Add MX Bank In Payment Methods</t>
+  </si>
+  <si>
+    <t>Payment Methods -  Mx Bank</t>
+  </si>
+  <si>
+    <t>Verify Buy Token with New and Existing MX Bank</t>
+  </si>
+  <si>
+    <t>Buy Token - MX Bank</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testDeleteBankAccount,
+-ppaymentHeading,
+-premovePopUpHeading,
+-ptoastMsg</t>
+  </si>
+  <si>
+    <t>Verify Withdraw Token with New and Existing Debit Cards</t>
+  </si>
+  <si>
+    <t>Withdraw Token - Debit Card</t>
+  </si>
+  <si>
+    <t>Verify Withdraw Token with New and Existing MX Bank</t>
+  </si>
+  <si>
+    <t>Withdraw Token - MX Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.CustomerProfileTest,
+testAddCards,
+-pcardHeading,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-pcvv,
+-ppreAuthHeading,
+-pcardSuccessHeading,
+-pcardSuccessDescription,
+-paddPaymentHeading,
+-ppreAuthiAmount,
+-ppaymentHeading
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.DashBoardTest,
+testBuyTokenWithCards,
+-ppaymentHeading,
+-pcardHeading,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-pcvv,
+-ppreAuthHeading,
+-paddPaymentHeading,
+-ptokensHeading,
+-ppreAuthiAmount,
+-pverifyBuyTokenWithExistingCard,
+-pcvvHeading,
+-pamount,
+-porderPopupHeading,
+-ppinHeading,
+-psuccessHeading,
+-psuccessDescription,
+-ppin,
+-pcardSuccessHeading,
+-pcardSuccessDescription
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.DashBoardTest,
+testWithdrawTokenWithCards,
+-pheading,
+-ppaymentHeading,
+-pcardHeading,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-pcvv,
+-ppreAuthHeading,
+-paddPaymentHeading,
+-ptokensHeading,
+-ppreAuthiAmount,
+-pverifyBuyTokenWithExistingCard,
+-pamount,
+-porderPopupHeading,
+-ppinHeading,
+-psuccessHeading,
+-psuccessDescription,
+-ppin,
+-pcardSuccessHeading,
+-pcardSuccessDescription,
+-pnoteMsg
+</t>
   </si>
   <si>
     <t>coyni_mobile.tests.CustomerProfileTest,
-testEditEmail,
+testBankAccount,
+-ppaymentHeading,
+-paddPaymentHeading,
+-pmxAddBankHeading,
+-pmxAddBankDescription,
+-pmxAddBankChkBxDescription,
+-pmxConfirmationHeading,
+-pmxConfirmationDescription,
+-pcredentialsHeading,
+-pmxUsername,
+-pmxPassword,
+-pcardSuccessHeading,
+-pcardSuccessDescription,
+-paccountType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.DashBoardTest,
+testBuyTokenWithBankAccount,
+-ppaymentHeading,
+-pheading,
+-paddPaymentHeading,
+-pmxAddBankHeading,
+-pmxAddBankDescription,
+-pmxAddBankChkBxDescription,
+-pmxConfirmationHeading,
+-pmxConfirmationDescription,
+-pcredentialsHeading,
+-pmxUsername,
+-pmxPassword,
+-ptokensHeading,
+-pverifyBuyTokenWithExistingCard,
+-pamount,
+-pnoteMsg,
+-porderPopupHeading,
 -ppinHeading,
+-psuccessHeading,
+-psuccessDescription,
+-ppin,
+-pcardSuccessHeading,
+-pcardSuccessDescription,
+-paccountType
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni_mobile.tests.DashBoardTest,
+testWithdrawTokenWithBankAccount,
+-ppaymentHeading,
+-pheading,
+-paddPaymentHeading,
+-pmxAddBankHeading,
+-pmxAddBankDescription,
+-pmxAddBankChkBxDescription,
+-pmxConfirmationHeading,
+-pmxConfirmationDescription,
+-pcredentialsHeading,
+-pmxUsername,
+-pmxPassword,
+-ptokensHeading,
+-pverifyBuyTokenWithExistingCard,
+-pamount,
+-pnoteMsg,
+-porderPopupHeading,
+-ppinHeading,
+-psuccessHeading,
+-psuccessDescription,
+-ppin,
+-pcardSuccessHeading,
+-pcardSuccessDescription,
+-paccountType
+</t>
+  </si>
+  <si>
+    <t>Verify Withdraw Token with Gift Cards</t>
+  </si>
+  <si>
+    <t>Withdraw Token - Gift Card</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testWithdrawGiftCard,
+-pheading,
+-pdescription,
+-ptokensHeading,
+-pamount,
+-pfirstName,
+-plastName,
 -pemail,
--pnewEmail,
--peditEmailHeading,
+-porderPopupHeading,
+-ppinHeading,
+-psuccessHeading,
 -ppin,
--pnewEmail,
--pcurrentEmailVerification,
--pcurrEmailVerifiDesc,
--pnewEmailVerifiDesc,
--pcode,
--pnewEmailVerification,
--psucessDesc,
--psucessHeading</t>
+-pvalidateVisaGiftCard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1185,6 +1532,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1206,7 +1559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1266,16 +1619,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1590,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1951,7 @@
     <col min="1" max="1" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="8" max="8" width="35.85546875" customWidth="1"/>
-    <col min="9" max="9" width="33" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1644,7 +1994,7 @@
     </row>
     <row r="2" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>45</v>
@@ -1670,7 +2020,7 @@
     </row>
     <row r="3" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>45</v>
@@ -1691,13 +2041,13 @@
         <v>47</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>45</v>
@@ -1718,12 +2068,12 @@
         <v>47</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>45</v>
@@ -1744,12 +2094,12 @@
         <v>75</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>45</v>
@@ -1770,12 +2120,12 @@
         <v>75</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>45</v>
@@ -1796,12 +2146,12 @@
         <v>75</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>45</v>
@@ -1822,12 +2172,12 @@
         <v>63</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>45</v>
@@ -1848,12 +2198,12 @@
         <v>63</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>45</v>
@@ -1874,12 +2224,12 @@
         <v>63</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>45</v>
@@ -1897,16 +2247,16 @@
         <v>16</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>45</v>
@@ -1924,16 +2274,16 @@
         <v>16</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>45</v>
@@ -1951,16 +2301,16 @@
         <v>16</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:12" ht="255" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>45</v>
@@ -1978,10 +2328,10 @@
         <v>16</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="I14" s="18"/>
     </row>
@@ -2008,14 +2358,14 @@
         <v>17</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>45</v>
@@ -2036,20 +2386,20 @@
         <v>17</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="204" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="204" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>15</v>
@@ -2061,24 +2411,24 @@
         <v>44</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="153" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>86</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>155</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>15</v>
@@ -2087,27 +2437,27 @@
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>69</v>
@@ -2119,24 +2469,24 @@
         <v>16</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>49</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>148</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>15</v>
@@ -2145,26 +2495,27 @@
         <v>16</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>51</v>
+        <v>86</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>151</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>15</v>
@@ -2176,25 +2527,24 @@
         <v>16</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>53</v>
+        <v>86</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>15</v>
@@ -2206,23 +2556,24 @@
         <v>16</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>15</v>
@@ -2234,25 +2585,24 @@
         <v>16</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>15</v>
@@ -2264,1182 +2614,1547 @@
         <v>16</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>58</v>
+        <v>115</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>60</v>
+        <v>99</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>62</v>
+        <v>115</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>15</v>
+        <v>115</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>65</v>
+        <v>16</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="225" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>68</v>
+        <v>16</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>72</v>
+      <c r="E29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I30" s="18"/>
-    </row>
-    <row r="31" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>77</v>
+        <v>115</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>113</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>80</v>
+        <v>21</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>81</v>
+      <c r="E32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>183</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>84</v>
+        <v>115</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="153" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="15">
-        <v>1</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>87</v>
+      <c r="E34" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I34" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>89</v>
+        <v>21</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="204" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>44</v>
+      <c r="E36" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>93</v>
       </c>
       <c r="H36" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="1:10" ht="293.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="1:10" ht="306" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="J41" s="19"/>
+    </row>
+    <row r="42" spans="1:10" ht="331.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="J43" s="19"/>
+    </row>
+    <row r="44" spans="1:10" ht="331.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" s="16"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H58" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="153" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="14" t="s">
+      <c r="I58" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="9" t="s">
+      <c r="E59" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H59" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I37" s="22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="15">
-        <v>1</v>
-      </c>
-      <c r="F38" s="15">
-        <v>2</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38" s="9" t="s">
+      <c r="I59" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I38" s="22" t="s">
+      <c r="I60" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I61" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="14" t="s">
+    <row r="62" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="H39" s="9" t="s">
+      <c r="E62" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H63" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I42" s="16" t="s">
+      <c r="I63" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I45" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G47" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>127</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I49" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I50" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+    <row r="64" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B64" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="11" t="s">
+      <c r="D64" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H51" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="H64" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="5" t="s">
+      <c r="B65" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="D65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
         <v>19</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H65" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="66" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="5" t="s">
+      <c r="B66" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="D66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
         <v>19</v>
       </c>
-      <c r="H53" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I53" s="10" t="s">
+      <c r="H66" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="67" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="5" t="s">
+      <c r="B67" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" t="s">
+      <c r="D67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I54" s="10" t="s">
+      <c r="H67" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I67" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="68" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>28</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="5" t="s">
+      <c r="B68" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="D68" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" t="s">
         <v>19</v>
       </c>
-      <c r="H55" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I55" s="10" t="s">
+      <c r="H68" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I68" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="69" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="5" t="s">
+      <c r="B69" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="D69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" t="s">
         <v>19</v>
       </c>
-      <c r="H56" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I56" s="10" t="s">
+      <c r="H69" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="70" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="5" t="s">
+      <c r="B70" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" t="s">
+      <c r="D70" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" t="s">
         <v>19</v>
       </c>
-      <c r="H57" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" s="10" t="s">
+      <c r="H70" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I70" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="71" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>33</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="5" t="s">
+      <c r="B71" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="D71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G71" t="s">
         <v>19</v>
       </c>
-      <c r="H58" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I58" s="10" t="s">
+      <c r="H71" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I71" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="72" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="5" t="s">
+      <c r="B72" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G59" t="s">
+      <c r="D72" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" t="s">
         <v>19</v>
       </c>
-      <c r="H59" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I59" s="10" t="s">
+      <c r="H72" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="73" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="5" t="s">
+      <c r="B73" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G60" t="s">
+      <c r="D73" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" t="s">
         <v>19</v>
       </c>
-      <c r="H60" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I60" s="10" t="s">
+      <c r="H73" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="74" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>37</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="5" t="s">
+      <c r="B74" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="D74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" t="s">
         <v>19</v>
       </c>
-      <c r="H61" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I61" s="10" t="s">
+      <c r="H74" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="75" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="5" t="s">
+      <c r="B75" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="6" t="s">
+      <c r="D75" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G75" t="s">
         <v>19</v>
       </c>
-      <c r="H62" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I62" s="10" t="s">
+      <c r="H75" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="76" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>38</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="5" t="s">
+      <c r="B76" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="6" t="s">
+      <c r="D76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G76" t="s">
         <v>19</v>
       </c>
-      <c r="H63" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I63" s="10" t="s">
+      <c r="H76" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="77" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="B77" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F64" s="6" t="s">
+      <c r="D77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G77" t="s">
         <v>19</v>
       </c>
-      <c r="H64" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="10" t="s">
+      <c r="H77" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I77" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E65" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F65" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G65" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H65" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Developed test methods for Filters
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\10-July-2023_v3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\19-July-2023_v3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E54F89-B5AC-446F-AF5E-61C788C18010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CD8B3E-D33B-47D2-823B-2A9B167A7FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="177">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1259,6 +1259,28 @@
 -premovePopUpHeading,
 -ptoastMsg,
 -paddPaymentHeading</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>testdata_3_0_customer.xls,filters</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.DashBoardTest,
+testFilters,
+-ptransactionHeading,
+-ptransDtlsHeading,
+-ptransactionType,
+-pfromAmount,
+-ptoAmount,
+-ptransactionType</t>
+  </si>
+  <si>
+    <t>Verify Filters with Transactions Types,Sub Types and Status</t>
   </si>
 </sst>
 </file>
@@ -1720,12 +1742,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="B52" sqref="B52"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2154,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
@@ -3474,6 +3496,37 @@
       <c r="K59" s="10" t="s">
         <v>159</v>
       </c>
+    </row>
+    <row r="60" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>174</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Modified the Test Scripts and Test Data for Customer Portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/03-Aug-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4255B0DD-D992-6B49-B0B9-399172EAEDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD65D48-7B17-B94D-9A4E-F8C376AEF79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -1900,10 +1900,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="B68" sqref="B68"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1967,7 +1967,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -3886,7 +3886,7 @@
         <v>146</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>19</v>
@@ -3895,7 +3895,7 @@
         <v>14</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Modified the Test Methods for Customer portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/03-Aug-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD65D48-7B17-B94D-9A4E-F8C376AEF79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBBF20A-A5FC-624B-BEE3-951E29E5F493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="195">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1094,9 +1094,6 @@
   </si>
   <si>
     <t>Scan Code</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>coyni_mobile.tests.DashBoardTest,
@@ -1900,10 +1897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1967,7 +1964,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1993,7 +1990,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>28</v>
@@ -2020,7 +2017,7 @@
         <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>28</v>
@@ -2046,7 +2043,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>28</v>
@@ -2072,7 +2069,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>28</v>
@@ -2098,7 +2095,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>28</v>
@@ -2124,7 +2121,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>28</v>
@@ -2150,7 +2147,7 @@
         <v>65</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>28</v>
@@ -2176,7 +2173,7 @@
         <v>68</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>28</v>
@@ -2202,7 +2199,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>28</v>
@@ -2229,7 +2226,7 @@
         <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>28</v>
@@ -2256,7 +2253,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>28</v>
@@ -2283,7 +2280,7 @@
         <v>75</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>28</v>
@@ -2310,7 +2307,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
@@ -2338,7 +2335,7 @@
         <v>79</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
@@ -2363,10 +2360,10 @@
     </row>
     <row r="17" spans="1:10" ht="371" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
@@ -2384,7 +2381,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="10"/>
@@ -2394,7 +2391,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>50</v>
@@ -2423,7 +2420,7 @@
         <v>89</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>50</v>
@@ -2452,7 +2449,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>50</v>
@@ -2481,7 +2478,7 @@
         <v>82</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>50</v>
@@ -2510,7 +2507,7 @@
         <v>85</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>50</v>
@@ -2539,7 +2536,7 @@
         <v>86</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>50</v>
@@ -2568,7 +2565,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>50</v>
@@ -2597,7 +2594,7 @@
         <v>111</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>50</v>
@@ -2626,7 +2623,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>50</v>
@@ -2655,7 +2652,7 @@
         <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>50</v>
@@ -2684,7 +2681,7 @@
         <v>96</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>50</v>
@@ -2713,7 +2710,7 @@
         <v>98</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>50</v>
@@ -2742,7 +2739,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>50</v>
@@ -2771,7 +2768,7 @@
         <v>42</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>50</v>
@@ -2800,7 +2797,7 @@
         <v>102</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>50</v>
@@ -2829,7 +2826,7 @@
         <v>104</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>50</v>
@@ -2858,7 +2855,7 @@
         <v>92</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>50</v>
@@ -2887,7 +2884,7 @@
         <v>52</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>50</v>
@@ -2916,7 +2913,7 @@
         <v>107</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>50</v>
@@ -2945,7 +2942,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>50</v>
@@ -2974,7 +2971,7 @@
         <v>150</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>116</v>
@@ -3000,10 +2997,10 @@
     </row>
     <row r="39" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>116</v>
@@ -3024,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="112" x14ac:dyDescent="0.2">
@@ -3032,7 +3029,7 @@
         <v>154</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>116</v>
@@ -3053,7 +3050,7 @@
         <v>20</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="224" x14ac:dyDescent="0.2">
@@ -3061,7 +3058,7 @@
         <v>153</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>116</v>
@@ -3087,10 +3084,10 @@
     </row>
     <row r="42" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>116</v>
@@ -3111,7 +3108,7 @@
         <v>20</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="112" x14ac:dyDescent="0.2">
@@ -3119,7 +3116,7 @@
         <v>155</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>116</v>
@@ -3140,15 +3137,15 @@
         <v>20</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="280" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>116</v>
@@ -3169,7 +3166,7 @@
         <v>20</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J44" s="19"/>
     </row>
@@ -3178,7 +3175,7 @@
         <v>114</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>116</v>
@@ -3205,10 +3202,10 @@
     </row>
     <row r="46" spans="1:10" ht="126" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>119</v>
@@ -3223,13 +3220,13 @@
         <v>25</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J46" s="19"/>
     </row>
@@ -3238,7 +3235,7 @@
         <v>118</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>119</v>
@@ -3259,10 +3256,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="224" x14ac:dyDescent="0.2">
@@ -3270,7 +3267,7 @@
         <v>114</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>116</v>
@@ -3297,10 +3294,10 @@
     </row>
     <row r="49" spans="1:12" ht="98" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>119</v>
@@ -3315,13 +3312,13 @@
         <v>15</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J49" s="19"/>
     </row>
@@ -3330,7 +3327,7 @@
         <v>125</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>119</v>
@@ -3351,16 +3348,18 @@
         <v>20</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="J50" s="19"/>
+        <v>169</v>
+      </c>
+      <c r="J50" s="19" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>116</v>
@@ -3387,10 +3386,10 @@
     </row>
     <row r="52" spans="1:12" ht="126" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>119</v>
@@ -3405,13 +3404,13 @@
         <v>15</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J52" s="19"/>
     </row>
@@ -3420,7 +3419,7 @@
         <v>122</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>119</v>
@@ -3441,7 +3440,7 @@
         <v>20</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J53" s="19" t="s">
         <v>124</v>
@@ -3452,7 +3451,7 @@
         <v>120</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>116</v>
@@ -3479,10 +3478,10 @@
     </row>
     <row r="55" spans="1:12" ht="98" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>119</v>
@@ -3497,13 +3496,13 @@
         <v>26</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J55" s="19"/>
     </row>
@@ -3512,7 +3511,7 @@
         <v>127</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>119</v>
@@ -3533,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J56" s="19" t="s">
         <v>124</v>
@@ -3544,7 +3543,7 @@
         <v>130</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>119</v>
@@ -3565,16 +3564,16 @@
         <v>20</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J57" s="19"/>
     </row>
     <row r="58" spans="1:12" ht="252" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>119</v>
@@ -3604,7 +3603,7 @@
         <v>21</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>19</v>
@@ -3631,7 +3630,7 @@
         <v>138</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="208" x14ac:dyDescent="0.2">
@@ -3639,7 +3638,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>19</v>
@@ -3669,7 +3668,7 @@
         <v>140</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>19</v>
@@ -3705,7 +3704,7 @@
         <v>142</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>19</v>
@@ -3741,7 +3740,7 @@
         <v>24</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>19</v>
@@ -3762,7 +3761,7 @@
         <v>20</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="192" x14ac:dyDescent="0.2">
@@ -3770,7 +3769,7 @@
         <v>23</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>19</v>
@@ -3791,7 +3790,7 @@
         <v>20</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="128" x14ac:dyDescent="0.2">
@@ -3799,7 +3798,7 @@
         <v>144</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>19</v>
@@ -3828,7 +3827,7 @@
         <v>24</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>19</v>
@@ -3849,7 +3848,7 @@
         <v>20</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="80" x14ac:dyDescent="0.2">
@@ -3857,7 +3856,7 @@
         <v>17</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>19</v>
@@ -3886,7 +3885,7 @@
         <v>146</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>19</v>
@@ -3921,7 +3920,7 @@
         <v>162</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>158</v>
@@ -3949,10 +3948,10 @@
     </row>
     <row r="70" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>158</v>
@@ -3967,13 +3966,13 @@
         <v>15</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>20</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>

</xml_diff>

<commit_message>
Modified the test data and test scripts files
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_3_0_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/03-Aug-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBBF20A-A5FC-624B-BEE3-951E29E5F493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F787418-7010-7C4C-90BB-5E6AE301F72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{019282C9-970D-47F1-9941-467340F5B535}"/>
   </bookViews>
@@ -1897,10 +1897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F9A69-EADA-47FB-8695-9464344F869C}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="J50" sqref="J50"/>
+      <selection pane="topRight" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>